<commit_message>
Bribery Victimization for West Caribbean
</commit_message>
<xml_diff>
--- a/Data/Methodology Summary_Andes 12.16.xlsx
+++ b/Data/Methodology Summary_Andes 12.16.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wjproject.sharepoint.com/research/Programmatic/Data Analytics/6. Country Reports/LAC-Reports/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="341" documentId="8_{D6C07217-55F6-40ED-9D1A-2B0BF938B636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30DA469F-BEAD-7547-978F-C6DAECEF6257}"/>
+  <xr:revisionPtr revIDLastSave="343" documentId="8_{D6C07217-55F6-40ED-9D1A-2B0BF938B636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC01A421-FAC5-1C40-85E9-5C1149FAB0FB}"/>
   <bookViews>
-    <workbookView xWindow="29100" yWindow="-21100" windowWidth="25480" windowHeight="21100" xr2:uid="{77AD0726-88D8-44DD-9080-F543DD60C64F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" activeTab="1" xr2:uid="{77AD0726-88D8-44DD-9080-F543DD60C64F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sampling Frame" sheetId="5" r:id="rId1"/>
-    <sheet name="AdminDivs" sheetId="6" r:id="rId2"/>
-    <sheet name="SampleDesc" sheetId="7" r:id="rId3"/>
-    <sheet name="Bolivia" sheetId="1" state="hidden" r:id="rId4"/>
-    <sheet name="Colombia" sheetId="2" state="hidden" r:id="rId5"/>
-    <sheet name="Ecuador" sheetId="3" state="hidden" r:id="rId6"/>
-    <sheet name="Peru" sheetId="4" state="hidden" r:id="rId7"/>
+    <sheet name="Hoja1" sheetId="8" r:id="rId2"/>
+    <sheet name="AdminDivs" sheetId="6" r:id="rId3"/>
+    <sheet name="SampleDesc" sheetId="7" r:id="rId4"/>
+    <sheet name="Bolivia" sheetId="1" state="hidden" r:id="rId5"/>
+    <sheet name="Colombia" sheetId="2" state="hidden" r:id="rId6"/>
+    <sheet name="Ecuador" sheetId="3" state="hidden" r:id="rId7"/>
+    <sheet name="Peru" sheetId="4" state="hidden" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="116">
   <si>
     <t>Sample Size</t>
   </si>
@@ -386,6 +387,9 @@
   </si>
   <si>
     <t>Sample Sub-Units 1</t>
+  </si>
+  <si>
+    <t>I&amp;QC</t>
   </si>
 </sst>
 </file>
@@ -861,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A370D2-6729-6642-9050-0182FD4A6CB8}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -993,6 +997,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9640C0A4-36A3-6E4D-ABDA-E66A7BC6C558}">
+  <dimension ref="C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="3:3">
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBD0801-F392-8E43-BE7F-67B3A843B1CB}">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -1276,7 +1300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B7FB5B-1ADA-344B-BEC0-179A66FAE9C7}">
   <dimension ref="A1:H72"/>
   <sheetViews>
@@ -2331,7 +2355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8924A71-BA49-4EF2-A583-E5C119517806}">
   <dimension ref="A1:D46"/>
   <sheetViews>
@@ -2580,7 +2604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B094D6-FCFF-4B3F-8157-EE7DA482D702}">
   <dimension ref="A1:E46"/>
   <sheetViews>
@@ -2864,7 +2888,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5646A9CD-758C-42C5-B58A-1B2FEF976F16}">
   <dimension ref="A1:D45"/>
   <sheetViews>
@@ -3153,7 +3177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{627D3E6B-CCDA-4A25-9566-3D28FC062E70}">
   <dimension ref="A1:G48"/>
   <sheetViews>
@@ -3560,6 +3584,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006BF094976B1C6245BAB5BCECAC284645" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="b17f52af6646b5583120346a68295973">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="69276225-f05c-44c5-92dc-c999460a4149" xmlns:ns3="46f3a809-46a3-44ee-a0f1-42a271529c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95a1201d1da507c70fe2596948b34472" ns2:_="" ns3:_="">
     <xsd:import namespace="69276225-f05c-44c5-92dc-c999460a4149"/>
@@ -3802,27 +3846,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A173B992-D409-46D4-A356-39CAA5E52A01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
+    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46f3a809-46a3-44ee-a0f1-42a271529c86">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="69276225-f05c-44c5-92dc-c999460a4149" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7423736F-E14C-4FBF-A48B-0B9C870C6645}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81DE00A8-7FD1-41B6-A6FD-F767B9DE5176}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3839,29 +3888,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7423736F-E14C-4FBF-A48B-0B9C870C6645}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A173B992-D409-46D4-A356-39CAA5E52A01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="69276225-f05c-44c5-92dc-c999460a4149"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="46f3a809-46a3-44ee-a0f1-42a271529c86"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>